<commit_message>
New RemoteGetDWG and RemoteGetFile files
New RemoteGetDWG and RemoteGetFile files

KMZ files pose many challenges, including decompressing the file,
choosing the correct KML file from the extracted files, etc. We attempt
to do this in the RemoteGetFile.java file.

We attempt to simplify this process by using DWG file instead, with
Class DWGParser.
</commit_message>
<xml_diff>
--- a/Marks/assign3.xlsx
+++ b/Marks/assign3.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\Markings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19140" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="16900" windowHeight="17380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -242,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -277,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,20 +489,20 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -552,7 +552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -579,7 +579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -606,7 +606,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -633,7 +633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -660,7 +660,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -687,7 +687,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -714,7 +714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -741,7 +741,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -768,7 +768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -795,7 +795,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -822,7 +822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -849,7 +849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -862,8 +862,8 @@
         <v>2</v>
       </c>
       <c r="H18">
-        <f>_xlfn.FLOOR.MATH(AVERAGE(G2:G13)*10)</f>
-        <v>56</v>
+        <f>AVERAGE(G2:G13)*10</f>
+        <v>56.666666666666671</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
@@ -872,7 +872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -889,7 +889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -906,13 +906,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21">
         <f>SUM(H18:H20)</f>
-        <v>86</v>
+        <v>86.666666666666671</v>
       </c>
       <c r="I21" t="s">
         <v>14</v>
@@ -923,6 +923,11 @@
     <mergeCell ref="B18:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -932,9 +937,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -944,8 +954,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>